<commit_message>
First drifing version (mid control)
</commit_message>
<xml_diff>
--- a/project/Projekt-Steuerung_Selbstfahrendes-Auto.xlsx
+++ b/project/Projekt-Steuerung_Selbstfahrendes-Auto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
     <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'PSP - WBS'!$A$3:$I$33</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'PSP - WBS'!$A$3:$I$34</definedName>
     <definedName function="false" hidden="false" name="Arbeitspaket" vbProcedure="false">[1]Stammdaten!$A$9:$A$10</definedName>
     <definedName function="false" hidden="false" name="Personen" vbProcedure="false">[1]Stammdaten!$A$27:$A$28</definedName>
     <definedName function="false" hidden="false" name="Prio" vbProcedure="false">[1]Stammdaten!$A$16:$A$18</definedName>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="232">
   <si>
     <t xml:space="preserve">Projekt: Selbstfahrendes Auto</t>
   </si>
@@ -806,12 +806,12 @@
     <t xml:space="preserve">Planungsaktivitäten laufend</t>
   </si>
   <si>
-    <t xml:space="preserve">Projektende</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aufsetzen Git Repository</t>
   </si>
   <si>
+    <t xml:space="preserve">Nur das Nötigste, Rest hier im Planungsexcel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bestellung und Auswahl 4WD-Car-Kits</t>
   </si>
   <si>
@@ -845,7 +845,13 @@
     <t xml:space="preserve">Konzept für Drehzahlmessung pro Motor überlegen</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementierung Drehzahlmessung</t>
+    <t xml:space="preserve">zusätzliche Hardware gekauft, Hall-Sensoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D-Druck für Sharp Sensoren Halterungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Stunden zeichnen, 1 Stunde drucken und anpassen</t>
   </si>
   <si>
     <t xml:space="preserve">Aufbau Sensorik</t>
@@ -854,7 +860,7 @@
     <t xml:space="preserve">Auswahl der Sensoren (4x Infrarot, 1x Ultraschall bereits vorhanden)</t>
   </si>
   <si>
-    <t xml:space="preserve">Vorerst keine weiteren Sensoren geplant</t>
+    <t xml:space="preserve">4x Infrarot entfernt, weil einfach nur Schrott, neue Sharp Sensoren besorgt</t>
   </si>
   <si>
     <t xml:space="preserve">Verkabelung + Positionierung der Sensoren</t>
@@ -867,67 +873,33 @@
     <t xml:space="preserve">Inbetriebnahme der Infrarotsensoren (inkl. sauberem leicht verwendbarem Interface zur Auswertung)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">06.02.2020
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">16.03.2020</t>
-    </r>
+    <t xml:space="preserve">cancelled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abgebrochen, Einstellung der Sensoren zu filigran, neue Sensoren gekauft</t>
   </si>
   <si>
     <t xml:space="preserve">Inbetriebnahme des Ultraschallsensors (inkl. sauberem leicht verwendbarem Interface zur Auswertung)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">06.02.2020
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">23.03.2020</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Funktioniert, aber delay + duration händisch hintereinander einzubauen → ev. Interrupt?</t>
+    <t xml:space="preserve">on hold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funktioniert, aber delay + duration händisch hintereinander einzubauen → ev. Interrupt?
+Derzeit on hold, da neue IR Sensoren</t>
   </si>
   <si>
     <t xml:space="preserve">Konzept + Inbetriebnahme der Servo-Ansteuerung (inkl. sauberem leicht verwendbarem Interface zur Positionierung)</t>
   </si>
   <si>
-    <t xml:space="preserve">Vergessen einzuplanen -&gt; beide Servos anzusteuern.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inbetriebnahme weiterer Sensoren</t>
+    <t xml:space="preserve">Vergessen einzuplanen -&gt; beide Servos anzusteuern.
+Derzeit on hold, da neue IR Sensoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verkabelung + Positionierung der Sharp Infrarot Sensoren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inbetriebnahme der Sharp Infrarotsensoren (inkl. sauberem leicht verwendbarem Interface zur Auswertung)</t>
   </si>
   <si>
     <t xml:space="preserve">Software Algorithmen</t>
@@ -936,90 +908,31 @@
     <t xml:space="preserve">Debugmöglichkeit überlegen (Bluetooth, LCD-Display, …)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10.02.2020
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">16.03.2020</t>
-    </r>
+    <t xml:space="preserve">LCD Display unpraktisch, da über die Entfernung nicht ablesbar</t>
   </si>
   <si>
     <t xml:space="preserve">Inbetriebnahme Debugmöglichkeit</t>
   </si>
   <si>
+    <t xml:space="preserve">Bluetooth App Inbetriebnahme hat länger gedauert – Fehler nicht gefunden, da für App anscheinend zu schnell übertragen
+Eine Aufzeichnungsmöglichkeit der Daten wird noch benötigt</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW-Konzept überlegen (Seitenregelung, Mittenregelung)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">12.02.2020
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">30.03.2020</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Implementierung Seitenregelung (inkl. Konfigurationsmöglichkeiten)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">16.02.2020
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">02.04.2020</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Implementierung Mittenregelung (inkl. Konfigurationsmöglichkeiten)</t>
   </si>
   <si>
+    <t xml:space="preserve">not in scope now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung Drehzahlmessung</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPL - Offene Punkte Liste</t>
   </si>
   <si>
@@ -1113,9 +1026,6 @@
     <t xml:space="preserve">Low</t>
   </si>
   <si>
-    <t xml:space="preserve">cancelled</t>
-  </si>
-  <si>
     <t xml:space="preserve">Risikoanalyse</t>
   </si>
   <si>
@@ -1275,7 +1185,10 @@
     <t xml:space="preserve">Aufgabe / Thema</t>
   </si>
   <si>
-    <t xml:space="preserve">Planung aktualisiert</t>
+    <t xml:space="preserve">Tagebuch erst späte begonnen (leider)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan ist, dass das Auto die erste Gerade schnell mittig fahren kann und die erste Kurve erkennt.</t>
   </si>
   <si>
     <t xml:space="preserve">Template</t>
@@ -1300,7 +1213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-C07]dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="_-[$€-C07]\ * #,##0.00_-;\-[$€-C07]\ * #,##0.00_-;_-[$€-C07]\ * \-??_-;_-@_-"/>
@@ -1309,8 +1222,9 @@
     <numFmt numFmtId="169" formatCode="General"/>
     <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="171" formatCode="@"/>
+    <numFmt numFmtId="172" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1389,14 +1303,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <strike val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -1427,7 +1333,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1438,6 +1344,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1909,48 +1821,44 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1969,20 +1877,20 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2005,15 +1913,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2145,7 +2053,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2245,9 +2157,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>94680</xdr:colOff>
+      <xdr:colOff>94320</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2260,13 +2172,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8308080" y="662760"/>
-          <a:ext cx="3071520" cy="2930400"/>
+          <a:off x="8309520" y="662760"/>
+          <a:ext cx="3076200" cy="2930040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2311,13 +2223,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -2628,8 +2540,8 @@
     <hyperlink ref="B18" r:id="rId6" display="https://github.com/philippjahn/car/research"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2639,17 +2551,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="132" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="132" width="36.77"/>
@@ -2658,32 +2570,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="133" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B1" s="133" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="132" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B2" s="132" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="132" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B3" s="132" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2692,17 +2604,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="37" width="58.87"/>
@@ -2903,8 +2815,8 @@
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2914,20 +2826,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3161,8 +3073,8 @@
     <mergeCell ref="A4:C4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3171,13 +3083,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3464,8 +3376,8 @@
     <hyperlink ref="F5" r:id="rId2" display="https://www.neuhold-elektronik.at/catshop/product_info.php?cPath=36_230&amp;products_id=7117"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3474,17 +3386,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.88"/>
@@ -3568,20 +3480,20 @@
         <v>3.5</v>
       </c>
       <c r="F5" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="75" t="s">
-        <v>99</v>
+        <v>2</v>
+      </c>
+      <c r="G5" s="75" t="n">
+        <v>44712</v>
       </c>
       <c r="H5" s="73"/>
       <c r="I5" s="76"/>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="n">
         <v>12</v>
       </c>
-      <c r="B6" s="72" t="s">
-        <v>100</v>
+      <c r="B6" s="77" t="s">
+        <v>99</v>
       </c>
       <c r="C6" s="73" t="s">
         <v>7</v>
@@ -3590,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="73" t="n">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="F6" s="73" t="n">
         <v>0</v>
@@ -3603,7 +3515,7 @@
       </c>
       <c r="I6" s="76"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="n">
         <v>13</v>
       </c>
@@ -3622,17 +3534,19 @@
       <c r="F7" s="73" t="n">
         <v>2.5</v>
       </c>
-      <c r="G7" s="75" t="s">
-        <v>99</v>
+      <c r="G7" s="75" t="n">
+        <v>44712</v>
       </c>
       <c r="H7" s="73"/>
-      <c r="I7" s="76"/>
+      <c r="I7" s="76" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="41" t="n">
         <v>14</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="77" t="s">
         <v>101</v>
       </c>
       <c r="C8" s="73" t="s">
@@ -3661,7 +3575,7 @@
       <c r="A9" s="41" t="n">
         <v>15</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="77" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="73" t="s">
@@ -3690,7 +3604,7 @@
       <c r="A10" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="72"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="73"/>
       <c r="D10" s="73"/>
       <c r="E10" s="73"/>
@@ -3700,7 +3614,7 @@
       <c r="I10" s="76"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="77" t="n">
+      <c r="A11" s="78" t="n">
         <v>20</v>
       </c>
       <c r="B11" s="69" t="s">
@@ -3718,7 +3632,7 @@
       <c r="A12" s="41" t="n">
         <v>21</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="77" t="s">
         <v>106</v>
       </c>
       <c r="C12" s="73" t="s">
@@ -3734,10 +3648,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="75" t="n">
-        <v>43863</v>
+        <v>44599</v>
       </c>
       <c r="H12" s="75" t="n">
-        <v>43832</v>
+        <v>44563</v>
       </c>
       <c r="I12" s="76" t="s">
         <v>107</v>
@@ -3747,7 +3661,7 @@
       <c r="A13" s="41" t="n">
         <v>22</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="77" t="s">
         <v>108</v>
       </c>
       <c r="C13" s="73" t="s">
@@ -3763,10 +3677,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="75" t="n">
-        <v>43864</v>
+        <v>44600</v>
       </c>
       <c r="H13" s="75" t="n">
-        <v>43833</v>
+        <v>44564</v>
       </c>
       <c r="I13" s="76"/>
     </row>
@@ -3774,7 +3688,7 @@
       <c r="A14" s="41" t="n">
         <v>23</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="77" t="s">
         <v>109</v>
       </c>
       <c r="C14" s="73" t="s">
@@ -3790,10 +3704,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="75" t="n">
-        <v>43865</v>
+        <v>44601</v>
       </c>
       <c r="H14" s="75" t="n">
-        <v>43835</v>
+        <v>44566</v>
       </c>
       <c r="I14" s="76"/>
     </row>
@@ -3801,7 +3715,7 @@
       <c r="A15" s="41" t="n">
         <v>24</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="77" t="s">
         <v>110</v>
       </c>
       <c r="C15" s="73" t="s">
@@ -3817,85 +3731,105 @@
         <v>0</v>
       </c>
       <c r="G15" s="75" t="n">
-        <v>43866</v>
+        <v>44602</v>
       </c>
       <c r="H15" s="75" t="n">
-        <v>43941</v>
+        <v>44612</v>
       </c>
       <c r="I15" s="76"/>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="78" t="n">
+    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="41" t="n">
         <v>25</v>
       </c>
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="81" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="76"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="78" t="n">
+      <c r="D16" s="74" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="75" t="n">
+        <v>44603</v>
+      </c>
+      <c r="H16" s="75" t="n">
+        <v>44615</v>
+      </c>
+      <c r="I16" s="76" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="41" t="n">
         <v>26</v>
       </c>
-      <c r="B17" s="79" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="80" t="s">
+      <c r="B17" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="81" t="n">
-        <v>12</v>
-      </c>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="76"/>
+      <c r="D17" s="74" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="73" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="75" t="n">
+        <v>44627</v>
+      </c>
+      <c r="H17" s="75" t="n">
+        <v>44627</v>
+      </c>
+      <c r="I17" s="76" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="72"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="73"/>
       <c r="D18" s="73"/>
       <c r="E18" s="73"/>
       <c r="F18" s="73"/>
       <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
+      <c r="H18" s="75"/>
       <c r="I18" s="76"/>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="77" t="n">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="78" t="n">
         <v>30</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C19" s="73"/>
       <c r="D19" s="73"/>
       <c r="E19" s="73"/>
       <c r="F19" s="73"/>
       <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
+      <c r="H19" s="75"/>
       <c r="I19" s="76"/>
     </row>
-    <row r="20" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="n">
         <v>31</v>
       </c>
-      <c r="B20" s="72" t="s">
-        <v>114</v>
+      <c r="B20" s="77" t="s">
+        <v>116</v>
       </c>
       <c r="C20" s="73" t="s">
         <v>7</v>
@@ -3904,27 +3838,27 @@
         <v>3</v>
       </c>
       <c r="E20" s="73" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F20" s="73" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="75" t="n">
-        <v>43866</v>
+        <v>44597</v>
       </c>
       <c r="H20" s="75" t="n">
-        <v>43833</v>
+        <v>44564</v>
       </c>
       <c r="I20" s="76" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="103.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="n">
         <v>32</v>
       </c>
-      <c r="B21" s="72" t="s">
-        <v>116</v>
+      <c r="B21" s="77" t="s">
+        <v>118</v>
       </c>
       <c r="C21" s="73" t="s">
         <v>7</v>
@@ -3945,15 +3879,15 @@
         <v>43833</v>
       </c>
       <c r="I21" s="76" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="41" t="n">
         <v>33</v>
       </c>
-      <c r="B22" s="72" t="s">
-        <v>118</v>
+      <c r="B22" s="77" t="s">
+        <v>120</v>
       </c>
       <c r="C22" s="73" t="s">
         <v>7</v>
@@ -3965,20 +3899,24 @@
         <v>3</v>
       </c>
       <c r="F22" s="73" t="n">
-        <v>4</v>
-      </c>
-      <c r="G22" s="82" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" s="73"/>
-      <c r="I22" s="76"/>
-    </row>
-    <row r="23" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="G22" s="75" t="n">
+        <v>44604</v>
+      </c>
+      <c r="H22" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="I22" s="76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="41" t="n">
         <v>34</v>
       </c>
-      <c r="B23" s="72" t="s">
-        <v>120</v>
+      <c r="B23" s="77" t="s">
+        <v>123</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>7</v>
@@ -3992,20 +3930,22 @@
       <c r="F23" s="73" t="n">
         <v>2</v>
       </c>
-      <c r="G23" s="82" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="75"/>
+      <c r="G23" s="75" t="n">
+        <v>44603</v>
+      </c>
+      <c r="H23" s="80" t="s">
+        <v>124</v>
+      </c>
       <c r="I23" s="76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="n">
         <v>35</v>
       </c>
-      <c r="B24" s="72" t="s">
-        <v>123</v>
+      <c r="B24" s="77" t="s">
+        <v>126</v>
       </c>
       <c r="C24" s="73" t="s">
         <v>7</v>
@@ -4019,250 +3959,318 @@
       <c r="F24" s="73" t="n">
         <v>4</v>
       </c>
-      <c r="G24" s="82" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" s="73"/>
+      <c r="G24" s="75" t="n">
+        <v>44603</v>
+      </c>
+      <c r="H24" s="80" t="s">
+        <v>124</v>
+      </c>
       <c r="I24" s="76" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="78" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="41" t="n">
         <v>36</v>
       </c>
-      <c r="B25" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="80" t="s">
+      <c r="B25" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
+      <c r="D25" s="74" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="75" t="n">
+        <v>44627</v>
+      </c>
+      <c r="H25" s="75" t="n">
+        <v>44627</v>
+      </c>
       <c r="I25" s="76"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41" t="s">
+    <row r="26" s="81" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="41" t="n">
+        <v>37</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="74" t="n">
+        <v>4</v>
+      </c>
+      <c r="E26" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="75" t="n">
+        <v>44634</v>
+      </c>
+      <c r="H26" s="75"/>
+      <c r="I26" s="76"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="76"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="77" t="n">
-        <v>40</v>
-      </c>
-      <c r="B27" s="69" t="s">
-        <v>126</v>
-      </c>
+      <c r="B27" s="77"/>
       <c r="C27" s="73"/>
       <c r="D27" s="73"/>
       <c r="E27" s="73"/>
       <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="76"/>
     </row>
-    <row r="28" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="83" t="n">
+    <row r="28" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="78" t="n">
+        <v>40</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="76"/>
+    </row>
+    <row r="29" s="81" customFormat="true" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="82" t="n">
         <v>41</v>
       </c>
-      <c r="B28" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="84" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="82" t="s">
-        <v>128</v>
-      </c>
-      <c r="H28" s="85"/>
-      <c r="I28" s="86"/>
-    </row>
-    <row r="29" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="B29" s="87" t="s">
-        <v>129</v>
+      <c r="B29" s="77" t="s">
+        <v>131</v>
       </c>
       <c r="C29" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="84" t="n">
-        <v>3</v>
-      </c>
-      <c r="E29" s="85" t="n">
+      <c r="D29" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="84" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="F29" s="85" t="n">
-        <v>3</v>
-      </c>
-      <c r="G29" s="82" t="s">
-        <v>128</v>
-      </c>
-      <c r="H29" s="85"/>
-      <c r="I29" s="86"/>
-    </row>
-    <row r="30" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="83" t="n">
-        <v>43</v>
-      </c>
-      <c r="B30" s="87" t="s">
-        <v>130</v>
+      <c r="G29" s="75" t="n">
+        <v>44634</v>
+      </c>
+      <c r="H29" s="75" t="n">
+        <v>44627</v>
+      </c>
+      <c r="I29" s="85" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" s="81" customFormat="true" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="82" t="n">
+        <v>42</v>
+      </c>
+      <c r="B30" s="86" t="s">
+        <v>133</v>
       </c>
       <c r="C30" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="84" t="n">
+      <c r="D30" s="83" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="E30" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="85" t="n">
+      <c r="F30" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="G30" s="82" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" s="85"/>
-      <c r="I30" s="86"/>
-    </row>
-    <row r="31" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="83" t="n">
-        <v>44</v>
-      </c>
-      <c r="B31" s="87" t="s">
-        <v>132</v>
+      <c r="G30" s="75" t="n">
+        <v>44634</v>
+      </c>
+      <c r="H30" s="75"/>
+      <c r="I30" s="85" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="82" t="n">
+        <v>43</v>
+      </c>
+      <c r="B31" s="86" t="s">
+        <v>135</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="84" t="n">
+      <c r="D31" s="83" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="84" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="75" t="n">
+        <v>44641</v>
+      </c>
+      <c r="H31" s="75"/>
+      <c r="I31" s="85"/>
+    </row>
+    <row r="32" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="82" t="n">
+        <v>44</v>
+      </c>
+      <c r="B32" s="86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="83" t="n">
         <v>6</v>
       </c>
-      <c r="E31" s="85" t="n">
+      <c r="E32" s="84" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="84" t="n">
+        <v>5</v>
+      </c>
+      <c r="G32" s="75" t="n">
+        <v>44648</v>
+      </c>
+      <c r="H32" s="75"/>
+      <c r="I32" s="85"/>
+    </row>
+    <row r="33" s="81" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="82" t="n">
+        <v>45</v>
+      </c>
+      <c r="B33" s="87" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="83" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="F31" s="85" t="n">
+      <c r="F33" s="84" t="n">
         <v>6</v>
       </c>
-      <c r="G31" s="82" t="s">
-        <v>133</v>
-      </c>
-      <c r="H31" s="85"/>
-      <c r="I31" s="86"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="88" t="n">
-        <v>45</v>
-      </c>
-      <c r="B32" s="89" t="s">
-        <v>134</v>
-      </c>
-      <c r="C32" s="80" t="s">
+      <c r="G33" s="75" t="n">
+        <v>44676</v>
+      </c>
+      <c r="H33" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="I33" s="85"/>
+    </row>
+    <row r="34" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="41" t="n">
+        <v>46</v>
+      </c>
+      <c r="B34" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="90" t="n">
-        <v>6</v>
-      </c>
-      <c r="E32" s="85"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="86"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="87"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="86"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="83"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="86"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="83"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="86"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="45"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
-      <c r="G36" s="92"/>
-      <c r="H36" s="92"/>
-      <c r="I36" s="93"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="66" t="n">
-        <f aca="false">SUM(D11:D36)</f>
-        <v>54</v>
-      </c>
-      <c r="E37" s="66" t="n">
-        <f aca="false">SUM(E11:E36)</f>
-        <v>20</v>
-      </c>
-      <c r="F37" s="66" t="n">
-        <f aca="false">SUM(F11:F36)</f>
-        <v>22</v>
-      </c>
-      <c r="I37" s="94"/>
+      <c r="D34" s="74" t="n">
+        <v>12</v>
+      </c>
+      <c r="E34" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="73" t="n">
+        <v>12</v>
+      </c>
+      <c r="G34" s="75" t="n">
+        <v>44683</v>
+      </c>
+      <c r="H34" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="I34" s="76"/>
+    </row>
+    <row r="35" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="82"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="85"/>
+    </row>
+    <row r="36" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="82"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="85"/>
+    </row>
+    <row r="37" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="45"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="91"/>
+      <c r="G37" s="91"/>
+      <c r="H37" s="91"/>
+      <c r="I37" s="92"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I38" s="94"/>
-    </row>
+      <c r="D38" s="66" t="n">
+        <f aca="false">SUM(D11:D37)</f>
+        <v>62</v>
+      </c>
+      <c r="E38" s="66" t="n">
+        <f aca="false">SUM(E11:E37)</f>
+        <v>38</v>
+      </c>
+      <c r="F38" s="66" t="n">
+        <f aca="false">SUM(F11:F37)</f>
+        <v>36</v>
+      </c>
+      <c r="I38" s="93"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="93"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A3:I33"/>
+  <autoFilter ref="A3:I34"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4273,13 +4281,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -4288,696 +4296,696 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="66" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="94" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="94" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="11.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="96" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="A1" s="95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3" s="97" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="98" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="97" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="97" t="s">
-        <v>140</v>
-      </c>
-      <c r="G3" s="97" t="s">
+      <c r="B3" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="C3" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="98" t="s">
+      <c r="D3" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="97" t="s">
+      <c r="E3" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="F3" s="96" t="s">
         <v>145</v>
       </c>
+      <c r="G3" s="96" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" s="97" t="s">
+        <v>148</v>
+      </c>
+      <c r="J3" s="96" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" s="96" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="99" t="n">
+      <c r="A4" s="98" t="n">
         <f aca="false">ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="B4" s="100" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="101" t="s">
+      <c r="B4" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="102" t="n">
+      <c r="D4" s="101" t="n">
         <v>43833</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="101" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" s="101" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" s="101" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="100" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="100" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="102" t="n">
+      <c r="I4" s="101" t="n">
         <v>43885</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="K4" s="103"/>
+        <v>155</v>
+      </c>
+      <c r="K4" s="102"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="104" t="n">
+      <c r="A5" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>2</v>
       </c>
-      <c r="B5" s="105" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="106" t="s">
+      <c r="B5" s="104" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="107" t="n">
+      <c r="D5" s="106" t="n">
         <v>43884</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="106" t="s">
-        <v>152</v>
-      </c>
-      <c r="G5" s="106" t="s">
-        <v>153</v>
-      </c>
-      <c r="H5" s="106" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="105" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="107" t="n">
+      <c r="I5" s="106" t="n">
         <v>43899</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="K5" s="108"/>
+        <v>159</v>
+      </c>
+      <c r="K5" s="107"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="104" t="n">
+      <c r="A6" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>3</v>
       </c>
-      <c r="B6" s="105" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="106" t="s">
+      <c r="B6" s="104" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="107" t="n">
+      <c r="D6" s="106" t="n">
         <v>43893</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="106" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="106" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="105" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="107" t="n">
+      <c r="I6" s="106" t="n">
         <v>43941</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="K6" s="108"/>
+        <v>162</v>
+      </c>
+      <c r="K6" s="107"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="104" t="n">
+      <c r="A7" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>4</v>
       </c>
-      <c r="B7" s="105" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="106" t="s">
+      <c r="B7" s="104" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="107" t="n">
+      <c r="D7" s="106" t="n">
         <v>43893</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="106" t="s">
-        <v>148</v>
-      </c>
-      <c r="G7" s="106" t="s">
-        <v>149</v>
-      </c>
-      <c r="H7" s="106" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="105" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="105" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="107" t="n">
+      <c r="I7" s="106" t="n">
         <v>43899</v>
       </c>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
     </row>
     <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="104" t="n">
+      <c r="A8" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>5</v>
       </c>
-      <c r="B8" s="104" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="106" t="s">
+      <c r="B8" s="103" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="107" t="n">
+      <c r="D8" s="106" t="n">
         <v>43920</v>
       </c>
-      <c r="E8" s="109" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" s="106" t="s">
-        <v>152</v>
-      </c>
-      <c r="G8" s="106" t="s">
-        <v>149</v>
-      </c>
-      <c r="H8" s="106" t="s">
+      <c r="E8" s="108" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="105" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="107" t="n">
+      <c r="I8" s="106" t="n">
         <v>43941</v>
       </c>
-      <c r="J8" s="108" t="s">
-        <v>160</v>
-      </c>
-      <c r="K8" s="108"/>
+      <c r="J8" s="107" t="s">
+        <v>165</v>
+      </c>
+      <c r="K8" s="107"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="104" t="n">
+      <c r="A9" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>6</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="107"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="106"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="107"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="104" t="n">
+      <c r="A10" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>7</v>
       </c>
-      <c r="B10" s="104"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="108"/>
-      <c r="K10" s="106"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="104" t="n">
+      <c r="A11" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>8</v>
       </c>
-      <c r="B11" s="104"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="106"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="105"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="104" t="n">
+      <c r="A12" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>9</v>
       </c>
-      <c r="B12" s="105"/>
-      <c r="C12" s="106"/>
-      <c r="D12" s="107"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="31"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="107"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="106"/>
       <c r="J12" s="31"/>
-      <c r="K12" s="106"/>
+      <c r="K12" s="105"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="104" t="n">
+      <c r="A13" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>10</v>
       </c>
-      <c r="B13" s="104"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="108"/>
-      <c r="K13" s="106"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="105"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="104" t="n">
+      <c r="A14" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>11</v>
       </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="108"/>
-      <c r="K14" s="108"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="106"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="107"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="104" t="n">
+      <c r="A15" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>12</v>
       </c>
-      <c r="B15" s="104"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="108"/>
-      <c r="K15" s="106"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="106"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="105"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="104" t="n">
+      <c r="A16" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>13</v>
       </c>
-      <c r="B16" s="104"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="106"/>
-      <c r="G16" s="106"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="106"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="105"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="104" t="n">
+      <c r="A17" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>14</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="108"/>
-      <c r="K17" s="106"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="105"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="104" t="n">
+      <c r="A18" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>15</v>
       </c>
-      <c r="B18" s="104"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="107"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="106"/>
-      <c r="K18" s="106"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="104" t="n">
+      <c r="A19" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>16</v>
       </c>
-      <c r="B19" s="104"/>
-      <c r="C19" s="106"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="107"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="106"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="105"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="107"/>
+      <c r="K19" s="105"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="104" t="n">
+      <c r="A20" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>17</v>
       </c>
-      <c r="B20" s="104"/>
-      <c r="C20" s="106"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="106"/>
-      <c r="G20" s="106"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="106"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="107"/>
+      <c r="K20" s="105"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="104" t="n">
+      <c r="A21" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>18</v>
       </c>
-      <c r="B21" s="104"/>
-      <c r="C21" s="106"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="106"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="106"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="105"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="104" t="n">
+      <c r="A22" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>19</v>
       </c>
-      <c r="B22" s="104"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="106"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="106"/>
-      <c r="I22" s="107"/>
-      <c r="J22" s="108"/>
-      <c r="K22" s="106"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="106"/>
+      <c r="J22" s="107"/>
+      <c r="K22" s="105"/>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="104" t="n">
+      <c r="A23" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>20</v>
       </c>
-      <c r="B23" s="104"/>
-      <c r="C23" s="106"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="107"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="106"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="107"/>
+      <c r="K23" s="105"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="104" t="n">
+      <c r="A24" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>21</v>
       </c>
-      <c r="B24" s="104"/>
-      <c r="C24" s="106"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="106"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="108"/>
-      <c r="K24" s="106"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="107"/>
+      <c r="K24" s="105"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="104" t="n">
+      <c r="A25" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>22</v>
       </c>
-      <c r="B25" s="104"/>
-      <c r="C25" s="106"/>
-      <c r="D25" s="107"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="108"/>
-      <c r="K25" s="106"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="107"/>
+      <c r="K25" s="105"/>
     </row>
     <row r="26" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="104" t="n">
+      <c r="A26" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>23</v>
       </c>
-      <c r="B26" s="104"/>
-      <c r="C26" s="106"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="106"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="108"/>
-      <c r="K26" s="106"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="106"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="105"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="104" t="n">
+      <c r="A27" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>24</v>
       </c>
-      <c r="B27" s="104"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="108"/>
-      <c r="K27" s="106"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="105"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="104" t="n">
+      <c r="A28" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>25</v>
       </c>
-      <c r="B28" s="104"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="108"/>
-      <c r="K28" s="106"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="106"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="105"/>
+      <c r="G28" s="105"/>
+      <c r="H28" s="105"/>
+      <c r="I28" s="106"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="105"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="104" t="n">
+      <c r="A29" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>26</v>
       </c>
-      <c r="B29" s="104"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="106"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="108"/>
-      <c r="K29" s="106"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="105"/>
+      <c r="I29" s="106"/>
+      <c r="J29" s="107"/>
+      <c r="K29" s="105"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="104" t="n">
+      <c r="A30" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>27</v>
       </c>
-      <c r="B30" s="104"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="107"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="106"/>
-      <c r="H30" s="106"/>
-      <c r="I30" s="107"/>
-      <c r="J30" s="108"/>
-      <c r="K30" s="106"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="105"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="105"/>
+      <c r="G30" s="105"/>
+      <c r="H30" s="105"/>
+      <c r="I30" s="106"/>
+      <c r="J30" s="107"/>
+      <c r="K30" s="105"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="104" t="n">
+      <c r="A31" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>28</v>
       </c>
-      <c r="B31" s="104"/>
-      <c r="C31" s="106"/>
-      <c r="D31" s="107"/>
-      <c r="E31" s="109"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
-      <c r="H31" s="106"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="108"/>
-      <c r="K31" s="106"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="105"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="105"/>
+      <c r="G31" s="105"/>
+      <c r="H31" s="105"/>
+      <c r="I31" s="106"/>
+      <c r="J31" s="107"/>
+      <c r="K31" s="105"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="104" t="n">
+      <c r="A32" s="103" t="n">
         <f aca="false">ROW()-3</f>
         <v>29</v>
       </c>
-      <c r="B32" s="104"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="107"/>
-      <c r="J32" s="108"/>
-      <c r="K32" s="106"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="106"/>
+      <c r="J32" s="107"/>
+      <c r="K32" s="105"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="110" t="n">
+      <c r="A33" s="109" t="n">
         <f aca="false">ROW()-3</f>
         <v>30</v>
       </c>
-      <c r="B33" s="110"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="111"/>
-      <c r="H33" s="111"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="114"/>
-      <c r="K33" s="111"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="110"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="113"/>
+      <c r="K33" s="110"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="66"/>
-      <c r="C34" s="115"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
-      <c r="J34" s="117"/>
-      <c r="K34" s="115"/>
+      <c r="C34" s="114"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="114"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="114"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="66"/>
-      <c r="C35" s="115"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="115"/>
-      <c r="G35" s="115"/>
-      <c r="H35" s="115"/>
-      <c r="J35" s="117"/>
-      <c r="K35" s="115"/>
+      <c r="C35" s="114"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="114"/>
+      <c r="G35" s="114"/>
+      <c r="H35" s="114"/>
+      <c r="J35" s="116"/>
+      <c r="K35" s="114"/>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G39" s="1" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E45" s="118"/>
+      <c r="E45" s="117"/>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="33"/>
@@ -4987,8 +4995,8 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5001,13 +5009,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5024,7 +5032,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -5042,25 +5050,25 @@
         <v>40</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5068,7 +5076,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C4" s="57" t="n">
         <v>4</v>
@@ -5076,13 +5084,13 @@
       <c r="D4" s="57" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="119" t="n">
+      <c r="E4" s="118" t="n">
         <f aca="false">C4*D4</f>
         <v>16</v>
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="31" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H4" s="31"/>
     </row>
@@ -5091,7 +5099,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C5" s="57" t="n">
         <v>1</v>
@@ -5099,7 +5107,7 @@
       <c r="D5" s="57" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="119" t="n">
+      <c r="E5" s="118" t="n">
         <f aca="false">C5*D5</f>
         <v>5</v>
       </c>
@@ -5112,11 +5120,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
-      <c r="E6" s="119" t="n">
+      <c r="E6" s="118" t="n">
         <f aca="false">C6*D6</f>
         <v>0</v>
       </c>
@@ -5129,11 +5137,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
-      <c r="E7" s="119" t="n">
+      <c r="E7" s="118" t="n">
         <f aca="false">C7*D7</f>
         <v>0</v>
       </c>
@@ -5148,7 +5156,7 @@
       <c r="B8" s="31"/>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
-      <c r="E8" s="119" t="n">
+      <c r="E8" s="118" t="n">
         <f aca="false">C8*D8</f>
         <v>0</v>
       </c>
@@ -5163,7 +5171,7 @@
       <c r="B9" s="31"/>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
-      <c r="E9" s="119" t="n">
+      <c r="E9" s="118" t="n">
         <f aca="false">C9*D9</f>
         <v>0</v>
       </c>
@@ -5178,7 +5186,7 @@
       <c r="B10" s="31"/>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
-      <c r="E10" s="119" t="n">
+      <c r="E10" s="118" t="n">
         <f aca="false">C10*D10</f>
         <v>0</v>
       </c>
@@ -5193,7 +5201,7 @@
       <c r="B11" s="31"/>
       <c r="C11" s="57"/>
       <c r="D11" s="57"/>
-      <c r="E11" s="119" t="n">
+      <c r="E11" s="118" t="n">
         <f aca="false">C11*D11</f>
         <v>0</v>
       </c>
@@ -5208,7 +5216,7 @@
       <c r="B12" s="31"/>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="119" t="n">
+      <c r="E12" s="118" t="n">
         <f aca="false">C12*D12</f>
         <v>0</v>
       </c>
@@ -5223,7 +5231,7 @@
       <c r="B13" s="31"/>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="119" t="n">
+      <c r="E13" s="118" t="n">
         <f aca="false">C13*D13</f>
         <v>0</v>
       </c>
@@ -5238,7 +5246,7 @@
       <c r="B14" s="31"/>
       <c r="C14" s="57"/>
       <c r="D14" s="57"/>
-      <c r="E14" s="119" t="n">
+      <c r="E14" s="118" t="n">
         <f aca="false">C14*D14</f>
         <v>0</v>
       </c>
@@ -5253,7 +5261,7 @@
       <c r="B15" s="31"/>
       <c r="C15" s="57"/>
       <c r="D15" s="57"/>
-      <c r="E15" s="119" t="n">
+      <c r="E15" s="118" t="n">
         <f aca="false">C15*D15</f>
         <v>0</v>
       </c>
@@ -5268,7 +5276,7 @@
       <c r="B16" s="31"/>
       <c r="C16" s="57"/>
       <c r="D16" s="57"/>
-      <c r="E16" s="119" t="n">
+      <c r="E16" s="118" t="n">
         <f aca="false">C16*D16</f>
         <v>0</v>
       </c>
@@ -5283,7 +5291,7 @@
       <c r="B17" s="31"/>
       <c r="C17" s="57"/>
       <c r="D17" s="57"/>
-      <c r="E17" s="119" t="n">
+      <c r="E17" s="118" t="n">
         <f aca="false">C17*D17</f>
         <v>0</v>
       </c>
@@ -5298,7 +5306,7 @@
       <c r="B18" s="31"/>
       <c r="C18" s="57"/>
       <c r="D18" s="57"/>
-      <c r="E18" s="119" t="n">
+      <c r="E18" s="118" t="n">
         <f aca="false">C18*D18</f>
         <v>0</v>
       </c>
@@ -5313,7 +5321,7 @@
       <c r="B19" s="31"/>
       <c r="C19" s="57"/>
       <c r="D19" s="57"/>
-      <c r="E19" s="119" t="n">
+      <c r="E19" s="118" t="n">
         <f aca="false">C19*D19</f>
         <v>0</v>
       </c>
@@ -5328,7 +5336,7 @@
       <c r="B20" s="31"/>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
-      <c r="E20" s="119" t="n">
+      <c r="E20" s="118" t="n">
         <f aca="false">C20*D20</f>
         <v>0</v>
       </c>
@@ -5343,7 +5351,7 @@
       <c r="B21" s="31"/>
       <c r="C21" s="57"/>
       <c r="D21" s="57"/>
-      <c r="E21" s="119" t="n">
+      <c r="E21" s="118" t="n">
         <f aca="false">C21*D21</f>
         <v>0</v>
       </c>
@@ -5358,7 +5366,7 @@
       <c r="B22" s="31"/>
       <c r="C22" s="57"/>
       <c r="D22" s="57"/>
-      <c r="E22" s="119" t="n">
+      <c r="E22" s="118" t="n">
         <f aca="false">C22*D22</f>
         <v>0</v>
       </c>
@@ -5373,7 +5381,7 @@
       <c r="B23" s="31"/>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
-      <c r="E23" s="119" t="n">
+      <c r="E23" s="118" t="n">
         <f aca="false">C23*D23</f>
         <v>0</v>
       </c>
@@ -5388,7 +5396,7 @@
       <c r="B24" s="31"/>
       <c r="C24" s="57"/>
       <c r="D24" s="57"/>
-      <c r="E24" s="119" t="n">
+      <c r="E24" s="118" t="n">
         <f aca="false">C24*D24</f>
         <v>0</v>
       </c>
@@ -5403,7 +5411,7 @@
       <c r="B25" s="31"/>
       <c r="C25" s="57"/>
       <c r="D25" s="57"/>
-      <c r="E25" s="119" t="n">
+      <c r="E25" s="118" t="n">
         <f aca="false">C25*D25</f>
         <v>0</v>
       </c>
@@ -5418,7 +5426,7 @@
       <c r="B26" s="31"/>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
-      <c r="E26" s="119" t="n">
+      <c r="E26" s="118" t="n">
         <f aca="false">C26*D26</f>
         <v>0</v>
       </c>
@@ -5433,7 +5441,7 @@
       <c r="B27" s="31"/>
       <c r="C27" s="57"/>
       <c r="D27" s="57"/>
-      <c r="E27" s="119" t="n">
+      <c r="E27" s="118" t="n">
         <f aca="false">C27*D27</f>
         <v>0</v>
       </c>
@@ -5448,7 +5456,7 @@
       <c r="B28" s="31"/>
       <c r="C28" s="57"/>
       <c r="D28" s="57"/>
-      <c r="E28" s="119" t="n">
+      <c r="E28" s="118" t="n">
         <f aca="false">C28*D28</f>
         <v>0</v>
       </c>
@@ -5463,7 +5471,7 @@
       <c r="B29" s="31"/>
       <c r="C29" s="57"/>
       <c r="D29" s="57"/>
-      <c r="E29" s="119" t="n">
+      <c r="E29" s="118" t="n">
         <f aca="false">C29*D29</f>
         <v>0</v>
       </c>
@@ -5478,7 +5486,7 @@
       <c r="B30" s="31"/>
       <c r="C30" s="57"/>
       <c r="D30" s="57"/>
-      <c r="E30" s="119" t="n">
+      <c r="E30" s="118" t="n">
         <f aca="false">C30*D30</f>
         <v>0</v>
       </c>
@@ -5493,7 +5501,7 @@
       <c r="B31" s="31"/>
       <c r="C31" s="57"/>
       <c r="D31" s="57"/>
-      <c r="E31" s="119" t="n">
+      <c r="E31" s="118" t="n">
         <f aca="false">C31*D31</f>
         <v>0</v>
       </c>
@@ -5508,7 +5516,7 @@
       <c r="B32" s="31"/>
       <c r="C32" s="57"/>
       <c r="D32" s="57"/>
-      <c r="E32" s="119" t="n">
+      <c r="E32" s="118" t="n">
         <f aca="false">C32*D32</f>
         <v>0</v>
       </c>
@@ -5523,7 +5531,7 @@
       <c r="B33" s="36"/>
       <c r="C33" s="58"/>
       <c r="D33" s="58"/>
-      <c r="E33" s="120" t="n">
+      <c r="E33" s="119" t="n">
         <f aca="false">C33*D33</f>
         <v>0</v>
       </c>
@@ -5548,8 +5556,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5559,17 +5567,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="25.11"/>
@@ -5577,302 +5585,302 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="121" t="s">
-        <v>179</v>
+      <c r="A1" s="120" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="122" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="123" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="123" t="s">
-        <v>184</v>
-      </c>
-      <c r="D4" s="123" t="s">
-        <v>185</v>
+      <c r="A4" s="121" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="122" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="122" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="122" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="123" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="124" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="123" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="124" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="124" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="124" t="s">
+        <v>193</v>
+      </c>
+      <c r="K6" s="125" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="123" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="124" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="124" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="124" t="s">
+        <v>200</v>
+      </c>
+      <c r="K7" s="121" t="s">
+        <v>201</v>
+      </c>
+      <c r="L7" s="121" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="121" t="s">
+        <v>203</v>
+      </c>
+      <c r="N7" s="121" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="123" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="124" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="124" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="124" t="s">
+        <v>207</v>
+      </c>
+      <c r="K8" s="123" t="s">
+        <v>199</v>
+      </c>
+      <c r="L8" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="M8" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="N8" s="123" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="123" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="K9" s="123" t="s">
+        <v>199</v>
+      </c>
+      <c r="L9" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="M9" s="123" t="s">
+        <v>200</v>
+      </c>
+      <c r="N9" s="123" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="123"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="124"/>
+      <c r="K10" s="123" t="s">
+        <v>206</v>
+      </c>
+      <c r="L10" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="M10" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="N10" s="123" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="123"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="K11" s="123" t="s">
+        <v>206</v>
+      </c>
+      <c r="L11" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="M11" s="123" t="s">
+        <v>200</v>
+      </c>
+      <c r="N11" s="123" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="123"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="K12" s="123" t="s">
+        <v>199</v>
+      </c>
+      <c r="L12" s="123" t="s">
+        <v>200</v>
+      </c>
+      <c r="M12" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="123" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="123"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="124"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="123"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="123"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="123"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="123"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="123"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="121" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="125" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="125" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="124" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="125" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="125" t="s">
-        <v>189</v>
-      </c>
-      <c r="K6" s="126" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="124" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" s="125" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>192</v>
-      </c>
-      <c r="D7" s="125" t="s">
-        <v>196</v>
-      </c>
-      <c r="K7" s="122" t="s">
-        <v>197</v>
-      </c>
-      <c r="L7" s="122" t="s">
-        <v>198</v>
-      </c>
-      <c r="M7" s="122" t="s">
-        <v>199</v>
-      </c>
-      <c r="N7" s="122" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="124" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="125" t="s">
-        <v>202</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="125" t="s">
-        <v>203</v>
-      </c>
-      <c r="K8" s="124" t="s">
-        <v>195</v>
-      </c>
-      <c r="L8" s="124" t="s">
-        <v>189</v>
-      </c>
-      <c r="M8" s="124" t="s">
-        <v>189</v>
-      </c>
-      <c r="N8" s="124" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="124" t="s">
+      <c r="B21" s="126" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="127" t="s">
         <v>205</v>
       </c>
-      <c r="B9" s="125"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="K9" s="124" t="s">
-        <v>195</v>
-      </c>
-      <c r="L9" s="124" t="s">
-        <v>189</v>
-      </c>
-      <c r="M9" s="124" t="s">
-        <v>196</v>
-      </c>
-      <c r="N9" s="124" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="124"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="K10" s="124" t="s">
-        <v>202</v>
-      </c>
-      <c r="L10" s="124" t="s">
-        <v>189</v>
-      </c>
-      <c r="M10" s="124" t="s">
-        <v>189</v>
-      </c>
-      <c r="N10" s="124" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="124"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="K11" s="124" t="s">
-        <v>202</v>
-      </c>
-      <c r="L11" s="124" t="s">
-        <v>189</v>
-      </c>
-      <c r="M11" s="124" t="s">
-        <v>196</v>
-      </c>
-      <c r="N11" s="124" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="124"/>
-      <c r="B12" s="125"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="K12" s="124" t="s">
-        <v>195</v>
-      </c>
-      <c r="L12" s="124" t="s">
-        <v>196</v>
-      </c>
-      <c r="M12" s="124" t="s">
-        <v>53</v>
-      </c>
-      <c r="N12" s="124" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="124"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="124"/>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="124"/>
-      <c r="B15" s="125"/>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="124"/>
-      <c r="B16" s="125"/>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="124"/>
-      <c r="B17" s="125"/>
-      <c r="C17" s="125"/>
-      <c r="D17" s="125"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="124"/>
-      <c r="B18" s="125"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="124"/>
-      <c r="B19" s="125"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="122" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="127" t="s">
-        <v>210</v>
-      </c>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="128" t="s">
-        <v>201</v>
-      </c>
-      <c r="B22" s="129" t="s">
-        <v>211</v>
-      </c>
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
+      <c r="B22" s="128" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="128" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23" s="129" t="s">
-        <v>213</v>
-      </c>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
+      <c r="A23" s="127" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="128" t="s">
+        <v>217</v>
+      </c>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="128" t="s">
-        <v>214</v>
-      </c>
-      <c r="B24" s="129" t="s">
-        <v>215</v>
-      </c>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
+      <c r="A24" s="127" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="128" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="124"/>
-      <c r="B25" s="130"/>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="124"/>
-      <c r="B26" s="130"/>
-      <c r="C26" s="130"/>
-      <c r="D26" s="130"/>
+      <c r="A26" s="123"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="124"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="130"/>
-      <c r="D27" s="130"/>
+      <c r="A27" s="123"/>
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="124"/>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="129"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="124"/>
-      <c r="B29" s="130"/>
-      <c r="C29" s="130"/>
-      <c r="D29" s="130"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5887,18 +5895,18 @@
     <mergeCell ref="B29:D29"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B5:B19" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B5:B19" type="list">
       <formula1>"sehr positiv,positiv,eher positiv,neutral,eher negativ,negativ,sehr negativ"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:D19" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:D19" type="list">
       <formula1>"sehr hoch,hoch,eher hoch,neutral,eher niedrig,niedrig,sehr niedrig"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5908,27 +5916,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="61.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="61.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="33" width="11.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -5936,30 +5944,36 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="53" t="n">
-        <v>43893</v>
-      </c>
-      <c r="B4" s="131" t="n">
-        <v>1</v>
+      <c r="A4" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="130" t="s">
+        <v>182</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="31"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="131" t="n">
+        <v>44634</v>
+      </c>
+      <c r="B5" s="57" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="57"/>
@@ -6106,8 +6120,8 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
displaycode added and minor improvements
</commit_message>
<xml_diff>
--- a/project/Projekt-Steuerung_Selbstfahrendes-Auto.xlsx
+++ b/project/Projekt-Steuerung_Selbstfahrendes-Auto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" state="visible" r:id="rId2"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="240">
   <si>
     <t xml:space="preserve">Projekt: Selbstfahrendes Auto</t>
   </si>
@@ -749,9 +749,15 @@
     <t xml:space="preserve">https://www.neuhold-elektronik.at/catshop/product_info.php?cPath=36_230&amp;products_id=7117</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.conrad.at/de/p/sony-us18650vtc5a-spezial-akku-18650-hochstromfaehig-flat-top-li-ion-3-7-v-2600-mah-1499575.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ladeschaltung für Li-Ion Akku</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.reichelt.at/at/de/entwicklerboards-ladeplatine-fuer-3-7v-li-akkus-usb-c-1a-debo1-3-7li-1-0a-p291398.html?&amp;nbc=1&amp;trstct=lsbght_sldr::114322</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kippschalter</t>
   </si>
   <si>
@@ -768,6 +774,24 @@
   </si>
   <si>
     <t xml:space="preserve">Eventuell 7805 Spannungsregler + hochohmige Widerstände für Batterieüberwachung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharp IR-Sensor 10-80cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.robotshop.com/de/de/sharp-gp2y0a21yk0f-ir-bereichssensor-10cm-bis-80cm.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharp IR-Sensor 20-150cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.robotshop.com/de/de/sharp-gp2y0a02yk0f-ir-entfernungssensor-20-cm-bis-150-cm.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumperkabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.conrad.at/de/p/whadda-wpa427-jumper-kabel-40x-drahtbruecken-stecker-40x-drahtbruecken-stecker-15-00-cm-bunt-2330813.html</t>
   </si>
   <si>
     <t xml:space="preserve">Summe</t>
@@ -1185,7 +1209,7 @@
     <t xml:space="preserve">Aufgabe / Thema</t>
   </si>
   <si>
-    <t xml:space="preserve">Tagebuch erst späte begonnen (leider)</t>
+    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">Plan ist, dass das Auto die erste Gerade schnell mittig fahren kann und die erste Kurve erkennt.</t>
@@ -2229,8 +2253,8 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2570,26 +2594,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="133" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B1" s="133" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="132" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B2" s="132" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="132" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B3" s="132" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3087,10 +3111,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3101,7 +3125,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="11.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="68.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="33" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="33" width="45.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="33" width="11.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3153,7 +3178,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="57" t="n">
         <v>2</v>
       </c>
@@ -3170,13 +3195,16 @@
       <c r="F5" s="62" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="57" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" s="57" t="n">
         <v>1</v>
@@ -3185,14 +3213,16 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="31"/>
-      <c r="F6" s="62"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="57" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C7" s="57" t="n">
         <v>1</v>
@@ -3201,23 +3231,24 @@
         <v>2</v>
       </c>
       <c r="E7" s="31"/>
+      <c r="F7" s="62"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="57" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D8" s="61" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,7 +3256,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C9" s="57" t="n">
         <v>1</v>
@@ -3235,7 +3266,7 @@
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,48 +3274,72 @@
         <v>9</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D10" s="61" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="61"/>
+      <c r="B11" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="57" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="61" t="n">
+        <v>16</v>
+      </c>
       <c r="E11" s="31"/>
-      <c r="F11" s="63"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="61"/>
+      <c r="B12" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="61" t="n">
+        <v>14</v>
+      </c>
       <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="61"/>
+      <c r="B13" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="61" t="n">
+        <v>5</v>
+      </c>
       <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="F13" s="31" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="57" t="n">
@@ -3359,12 +3414,12 @@
     <row r="21" s="59" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="64"/>
       <c r="B21" s="59" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C21" s="64"/>
       <c r="D21" s="65" t="n">
         <f aca="false">SUM(D4:D20)</f>
-        <v>45.5</v>
+        <v>80.5</v>
       </c>
     </row>
   </sheetData>
@@ -3374,6 +3429,7 @@
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="https://www.banggood.com/de/4WD-DIY-Smart-Chassis-Car-Kit-For-Arduino-with-UNO-R3-Ultrasonic-ModuleMotor-drive-board-p-1332912.html?akmClientCountry=AT&amp;rmmds=detail-left-hotproducts__4&amp;cur_warehouse=CN"/>
     <hyperlink ref="F5" r:id="rId2" display="https://www.neuhold-elektronik.at/catshop/product_info.php?cPath=36_230&amp;products_id=7117"/>
+    <hyperlink ref="F6" r:id="rId3" display="https://www.reichelt.at/at/de/entwicklerboards-ladeplatine-fuer-3-7v-li-akkus-usb-c-1a-debo1-3-7li-1-0a-p291398.html?&amp;nbc=1&amp;trstct=lsbght_sldr::114322"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3408,7 +3464,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3424,28 +3480,28 @@
         <v>40</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C3" s="67" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D3" s="67" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E3" s="67" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F3" s="67" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G3" s="67" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="H3" s="67" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="I3" s="67" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3453,7 +3509,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C4" s="70"/>
       <c r="D4" s="70"/>
@@ -3468,7 +3524,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C5" s="73" t="s">
         <v>7</v>
@@ -3493,7 +3549,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="77" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C6" s="73" t="s">
         <v>7</v>
@@ -3539,7 +3595,7 @@
       </c>
       <c r="H7" s="73"/>
       <c r="I7" s="76" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3547,7 +3603,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="77" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C8" s="73" t="s">
         <v>7</v>
@@ -3568,7 +3624,7 @@
         <v>44166</v>
       </c>
       <c r="I8" s="76" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3576,7 +3632,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="77" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C9" s="73" t="s">
         <v>7</v>
@@ -3597,7 +3653,7 @@
         <v>43885</v>
       </c>
       <c r="I9" s="76" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3674,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C11" s="73"/>
       <c r="D11" s="73"/>
@@ -3633,7 +3689,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>7</v>
@@ -3654,7 +3710,7 @@
         <v>44563</v>
       </c>
       <c r="I12" s="76" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,7 +3718,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="77" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C13" s="73" t="s">
         <v>7</v>
@@ -3689,7 +3745,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="77" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C14" s="73" t="s">
         <v>7</v>
@@ -3716,7 +3772,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="77" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C15" s="73" t="s">
         <v>7</v>
@@ -3743,7 +3799,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="77" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C16" s="73" t="s">
         <v>7</v>
@@ -3764,7 +3820,7 @@
         <v>44615</v>
       </c>
       <c r="I16" s="76" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3772,7 +3828,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="77" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>7</v>
@@ -3793,7 +3849,7 @@
         <v>44627</v>
       </c>
       <c r="I17" s="76" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,7 +3870,7 @@
         <v>30</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C19" s="73"/>
       <c r="D19" s="73"/>
@@ -3829,7 +3885,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="77" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C20" s="73" t="s">
         <v>7</v>
@@ -3850,7 +3906,7 @@
         <v>44564</v>
       </c>
       <c r="I20" s="76" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="103.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3858,7 +3914,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="77" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C21" s="73" t="s">
         <v>7</v>
@@ -3879,7 +3935,7 @@
         <v>43833</v>
       </c>
       <c r="I21" s="76" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3887,7 +3943,7 @@
         <v>33</v>
       </c>
       <c r="B22" s="77" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C22" s="73" t="s">
         <v>7</v>
@@ -3905,10 +3961,10 @@
         <v>44604</v>
       </c>
       <c r="H22" s="79" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="I22" s="76" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3916,7 +3972,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>7</v>
@@ -3934,10 +3990,10 @@
         <v>44603</v>
       </c>
       <c r="H23" s="80" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="I23" s="76" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,7 +4001,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="77" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C24" s="73" t="s">
         <v>7</v>
@@ -3963,10 +4019,10 @@
         <v>44603</v>
       </c>
       <c r="H24" s="80" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="I24" s="76" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3974,7 +4030,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="77" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C25" s="73" t="s">
         <v>7</v>
@@ -4001,7 +4057,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="72" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C26" s="73" t="s">
         <v>7</v>
@@ -4039,7 +4095,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
@@ -4054,7 +4110,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="77" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C29" s="73" t="s">
         <v>7</v>
@@ -4075,7 +4131,7 @@
         <v>44627</v>
       </c>
       <c r="I29" s="85" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" s="81" customFormat="true" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4083,7 +4139,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="86" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C30" s="73" t="s">
         <v>7</v>
@@ -4102,7 +4158,7 @@
       </c>
       <c r="H30" s="75"/>
       <c r="I30" s="85" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4110,7 +4166,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="86" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>7</v>
@@ -4135,7 +4191,7 @@
         <v>44</v>
       </c>
       <c r="B32" s="86" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C32" s="73" t="s">
         <v>7</v>
@@ -4160,7 +4216,7 @@
         <v>45</v>
       </c>
       <c r="B33" s="87" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C33" s="73" t="s">
         <v>7</v>
@@ -4178,7 +4234,7 @@
         <v>44676</v>
       </c>
       <c r="H33" s="80" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="I33" s="85"/>
     </row>
@@ -4187,7 +4243,7 @@
         <v>46</v>
       </c>
       <c r="B34" s="88" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C34" s="73" t="s">
         <v>7</v>
@@ -4205,7 +4261,7 @@
         <v>44683</v>
       </c>
       <c r="H34" s="80" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="I34" s="76"/>
     </row>
@@ -4309,7 +4365,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="95" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -4328,34 +4384,34 @@
         <v>40</v>
       </c>
       <c r="B3" s="96" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C3" s="96" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D3" s="97" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E3" s="96" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F3" s="96" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="G3" s="96" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="H3" s="96" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="I3" s="97" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="J3" s="96" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="K3" s="96" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4364,7 +4420,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C4" s="100" t="s">
         <v>7</v>
@@ -4373,13 +4429,13 @@
         <v>43833</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F4" s="100" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G4" s="100" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H4" s="100" t="s">
         <v>7</v>
@@ -4388,7 +4444,7 @@
         <v>43885</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="K4" s="102"/>
     </row>
@@ -4398,7 +4454,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="104" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C5" s="105" t="s">
         <v>7</v>
@@ -4407,13 +4463,13 @@
         <v>43884</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="F5" s="105" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="G5" s="105" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="H5" s="105" t="s">
         <v>7</v>
@@ -4422,7 +4478,7 @@
         <v>43899</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K5" s="107"/>
     </row>
@@ -4432,7 +4488,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="104" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C6" s="105" t="s">
         <v>7</v>
@@ -4441,13 +4497,13 @@
         <v>43893</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="F6" s="105" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="G6" s="105" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="H6" s="105" t="s">
         <v>7</v>
@@ -4456,7 +4512,7 @@
         <v>43941</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="K6" s="107"/>
     </row>
@@ -4466,7 +4522,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="104" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C7" s="105" t="s">
         <v>7</v>
@@ -4475,13 +4531,13 @@
         <v>43893</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="F7" s="105" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G7" s="105" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H7" s="105" t="s">
         <v>7</v>
@@ -4498,7 +4554,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="103" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C8" s="105" t="s">
         <v>7</v>
@@ -4507,13 +4563,13 @@
         <v>43920</v>
       </c>
       <c r="E8" s="108" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="F8" s="105" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="G8" s="105" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H8" s="105" t="s">
         <v>7</v>
@@ -4522,7 +4578,7 @@
         <v>43941</v>
       </c>
       <c r="J8" s="107" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="K8" s="107"/>
     </row>
@@ -4948,40 +5004,40 @@
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G39" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5032,7 +5088,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -5050,25 +5106,25 @@
         <v>40</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5076,7 +5132,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C4" s="57" t="n">
         <v>4</v>
@@ -5090,7 +5146,7 @@
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="31" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H4" s="31"/>
     </row>
@@ -5099,7 +5155,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C5" s="57" t="n">
         <v>1</v>
@@ -5120,7 +5176,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
@@ -5137,7 +5193,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
@@ -5586,134 +5642,134 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="120" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="121" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B4" s="122" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C4" s="122" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D4" s="122" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="123" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B5" s="124" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D5" s="124" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="123" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D6" s="124" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="K6" s="125" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="123" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B7" s="124" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D7" s="124" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="K7" s="121" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="L7" s="121" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="M7" s="121" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="N7" s="121" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="123" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B8" s="124" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D8" s="124" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="K8" s="123" t="s">
-        <v>199</v>
-      </c>
       <c r="L8" s="123" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="M8" s="123" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="N8" s="123" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="123" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B9" s="124"/>
       <c r="C9" s="124"/>
       <c r="D9" s="124"/>
       <c r="K9" s="123" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="L9" s="123" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="M9" s="123" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="N9" s="123" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5722,16 +5778,16 @@
       <c r="C10" s="124"/>
       <c r="D10" s="124"/>
       <c r="K10" s="123" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="L10" s="123" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="M10" s="123" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="N10" s="123" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5740,16 +5796,16 @@
       <c r="C11" s="124"/>
       <c r="D11" s="124"/>
       <c r="K11" s="123" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="L11" s="123" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="M11" s="123" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="N11" s="123" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5758,16 +5814,16 @@
       <c r="C12" s="124"/>
       <c r="D12" s="124"/>
       <c r="K12" s="123" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="L12" s="123" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="M12" s="123" t="s">
         <v>53</v>
       </c>
       <c r="N12" s="123" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,40 +5870,40 @@
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="121" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B21" s="126" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C21" s="126"/>
       <c r="D21" s="126"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="127" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B22" s="128" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C22" s="128"/>
       <c r="D22" s="128"/>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="127" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B23" s="128" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C23" s="128"/>
       <c r="D23" s="128"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="127" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B24" s="128" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C24" s="128"/>
       <c r="D24" s="128"/>
@@ -5922,7 +5978,7 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5936,7 +5992,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -5944,24 +6000,24 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="53" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B4" s="130" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5972,7 +6028,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>